<commit_message>
added correct smn2 cipher
</commit_message>
<xml_diff>
--- a/cluster/analysis_smn2_cipher/metadata_smn2_cipher.xlsx
+++ b/cluster/analysis_smn2_cipher/metadata_smn2_cipher.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkinney/github/22_drugs/cluster/analysis_smn2_cipher/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E3C666-6799-4B42-ACF0-B3A5DC214162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCF82DC-A83F-E544-A2AF-7C206A3957F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="11980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13040" yWindow="2820" windowWidth="41260" windowHeight="26660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIDs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>LID</t>
   </si>
@@ -43,10 +43,10 @@
     <t>description</t>
   </si>
   <si>
-    <t>304987001_smn2_ssbc_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>NONE</t>
+    <t>306771_ssbc_S1_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>306771_ssbc_S1_R2_001.fastq.gz</t>
   </si>
   <si>
     <t>smn2_ssbc</t>
@@ -73,25 +73,25 @@
     <t>features</t>
   </si>
   <si>
-    <t>smn2_5sslib_ssbc_lib1</t>
-  </si>
-  <si>
     <t>TAAGTGGCGC</t>
   </si>
   <si>
-    <t>smn2_5sslib_ssbc_read1</t>
-  </si>
-  <si>
-    <t>smn2_5sslib_ssbc_read2</t>
-  </si>
-  <si>
     <t>ss, bc</t>
   </si>
   <si>
-    <t>smn2_5sslib_ssbc_lib2</t>
-  </si>
-  <si>
-    <t>ATGCTCAGTA</t>
+    <t>CCATGCCAC</t>
+  </si>
+  <si>
+    <t>AAGCATCA</t>
+  </si>
+  <si>
+    <t>TCTGAGC</t>
+  </si>
+  <si>
+    <t>AACTAAGCCT</t>
+  </si>
+  <si>
+    <t>CGGATTCAG</t>
   </si>
   <si>
     <t>read</t>
@@ -103,16 +103,16 @@
     <t>sequence</t>
   </si>
   <si>
-    <t>.*CTTAAATTAA(?P&lt;ss&gt;.{9})CTGCCAGCAT.*GCATTCTAGA(?P&lt;bc&gt;.{20})GCGGCCGC.*</t>
-  </si>
-  <si>
-    <t>GTGCTCACATTCCTTAAATTAANNNGYNNNNCTGCCAGCATGCAGGTGGATGCACATGATGACATAATCACCTGCATTCTAGANNNNNNNNNNNNNNNNNNNNGCGGCCGCGCGCCACTTAAGATCGGAAGAGCGGTTCAGCAGGAATGC</t>
-  </si>
-  <si>
-    <t>.*GCGGCCGC(?P&lt;bc_rc&gt;.{20})TCTAGAATGC.*ATGCTGGCAG(?P&lt;ss_rc&gt;.{9})TTAATTTAAG.*</t>
-  </si>
-  <si>
-    <t>GCGGCCGCNNNNNNNNNNNNNNNNNNNNTCTAGAATGCAGGTGATTATGTCATCATGTGCATCCACCTGCATGCTGGCAGNNNNRCNNNTTAATTTAAGGAATGTGAGCACGCGCCACTTAAGATCGGAAGAGCGTCGTGTAGGGAAAGA</t>
+    <t>.*CTTAAATTA(?P&lt;ss&gt;.{10})CTGCCAGCAT.*</t>
+  </si>
+  <si>
+    <t>GTGCTCACATTCCTTAAATTANNNNGYNNNNCTGCCAGCATGCAGGTGGATGCACATGATGACATAATCACCTGCATTCTAGANNNNNNNNNNNNNNNNNNNNGCGGCCGCGCGCCACTTAAGATCGGAAGAGCGGTTCAGCAGGAATGC</t>
+  </si>
+  <si>
+    <t>.*GCGGCCGC(?P&lt;bc_rc&gt;.{20})TCTAGAATGC.*</t>
+  </si>
+  <si>
+    <t>GCGGCCGCNNNNNNNNNNNNNNNNNNNNTCTAGAATGCAGGTGATTATGTCATCATGTGCATCCACCTGCATGCTGGCAGNNNNRCNNNNTAATTTAAGGAATGTGAGCACGCGCCACTTAAGATCGGAAGAGCGTCGTGTAGGGAAAGA</t>
   </si>
   <si>
     <t>experiment</t>
@@ -124,19 +124,67 @@
     <t>file</t>
   </si>
   <si>
-    <t>smn2_lib1</t>
-  </si>
-  <si>
     <t>cipher</t>
   </si>
   <si>
-    <t>./cipher/cipher.smn2_5sslib_ssbc_lib1.txt</t>
-  </si>
-  <si>
-    <t>smn2_lib2</t>
-  </si>
-  <si>
-    <t>./cipher/cipher.smn2_5sslib_ssbc_lib2.txt</t>
+    <t>smn2_ssbc_lib1</t>
+  </si>
+  <si>
+    <t>smn2_ssbc_read1</t>
+  </si>
+  <si>
+    <t>smn2_ssbc_read2</t>
+  </si>
+  <si>
+    <t>smn2_ssbc_lib2</t>
+  </si>
+  <si>
+    <t>smn2_ssbc_lib3</t>
+  </si>
+  <si>
+    <t>smn2_ssbc_lib4</t>
+  </si>
+  <si>
+    <t>smn2_ssbc_lib5</t>
+  </si>
+  <si>
+    <t>smn2_ssbc_lib6</t>
+  </si>
+  <si>
+    <t>smn2_lib1_rep1</t>
+  </si>
+  <si>
+    <t>./cipher/cipher.smn2_ssbc_lib1.txt</t>
+  </si>
+  <si>
+    <t>smn2_lib1_rep2</t>
+  </si>
+  <si>
+    <t>smn2_lib1_rep3</t>
+  </si>
+  <si>
+    <t>smn2_lib2_rep1</t>
+  </si>
+  <si>
+    <t>./cipher/cipher.smn2_ssbc_lib4.txt</t>
+  </si>
+  <si>
+    <t>smn2_lib2_rep2</t>
+  </si>
+  <si>
+    <t>smn2_lib2_rep3</t>
+  </si>
+  <si>
+    <t>smn2_lib3_rep1</t>
+  </si>
+  <si>
+    <t>./cipher/cipher.smn2_ssbc_lib6.txt</t>
+  </si>
+  <si>
+    <t>smn2_lib3_rep2</t>
+  </si>
+  <si>
+    <t>smn2_lib3_rep3</t>
   </si>
 </sst>
 </file>
@@ -155,7 +203,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -163,20 +211,20 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Courier New"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -202,7 +250,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -220,16 +268,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView zoomScale="178" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,7 +584,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -543,8 +592,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>304987001</v>
+      <c r="A2" s="1">
+        <v>306771</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
@@ -552,26 +601,33 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="12">
-        <v>43749</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="11">
+        <v>44065</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="3"/>
@@ -632,24 +688,6 @@
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C54" s="3"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C55" s="3"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C56" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -658,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,391 +744,705 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1">
+        <v>306771</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="3">
-        <v>304987001</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="b">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1">
+        <v>306771</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1">
+        <v>306771</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1">
+        <v>306771</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1">
+        <v>306771</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3">
-        <v>304987001</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1">
+        <v>306771</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="b">
+      <c r="D7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="E10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="E11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="E12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="E13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="E14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
-      <c r="C29" s="10"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
-      <c r="C30" s="10"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E30" s="9"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
-      <c r="C31" s="10"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E31" s="9"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
-      <c r="C32" s="10"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="E32" s="9"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
-      <c r="C33" s="10"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="E33" s="9"/>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-      <c r="C34" s="10"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="I34" s="7"/>
+      <c r="E34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
-      <c r="C35" s="10"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="E35" s="9"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
-      <c r="C36" s="10"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="I36" s="7"/>
+      <c r="E36" s="9"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
-      <c r="C37" s="10"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="I37" s="7"/>
+      <c r="E37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="7"/>
+      <c r="E38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="7"/>
+      <c r="E39" s="9"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="7"/>
+      <c r="E40" s="9"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="7"/>
+      <c r="E43" s="9"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="7"/>
+      <c r="E44" s="9"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="7"/>
+      <c r="E45" s="9"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="7"/>
+      <c r="E46" s="9"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="7"/>
+      <c r="E47" s="9"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E48" s="9"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="7"/>
-    </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E49" s="9"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E50" s="9"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E51" s="9"/>
+      <c r="G51" s="9"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="7"/>
-    </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="7"/>
-    </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="7"/>
-    </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="7"/>
+      <c r="E52" s="9"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="I63" s="9"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="I66" s="9"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="I67" s="9"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="I68" s="9"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="I69" s="9"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="I70" s="9"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="I71" s="9"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="I72" s="9"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="9"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="9"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="9"/>
+    </row>
+    <row r="82" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="9"/>
+    </row>
+    <row r="83" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="9"/>
+    </row>
+    <row r="84" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="9"/>
+    </row>
+    <row r="85" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="9"/>
+    </row>
+    <row r="86" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="9"/>
+    </row>
+    <row r="87" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="9"/>
+    </row>
+    <row r="88" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="9"/>
+    </row>
+    <row r="89" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="9"/>
+    </row>
+    <row r="90" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1100,18 +1452,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+    <sheetView zoomScale="134" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="45" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="209" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="20" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45" style="1"/>
+    <col min="3" max="3" width="163.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="45" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1127,7 +1479,7 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
@@ -1138,7 +1490,7 @@
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>28</v>
@@ -1147,41 +1499,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
       <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="9"/>
+      <c r="C7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1190,15 +1526,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="45.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
@@ -1217,46 +1553,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
     </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+    </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>